<commit_message>
Ajustement de la navigation entre les pages
</commit_message>
<xml_diff>
--- a/CalculControlerButtonsState.xlsx
+++ b/CalculControlerButtonsState.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo-\source\repos\Depot_ProjetSynthese\420-W57-SF_E23_4394_TrackSense_AppEmbarque\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4172C51-89BF-4E1E-86D9-4C51CBD24F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15E6C54-A15E-4065-A7C7-EC45F0217E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{AEE4271D-9535-4907-B2D0-C9C19E933E7B}"/>
+    <workbookView xWindow="-28920" yWindow="10620" windowWidth="29040" windowHeight="15720" xr2:uid="{AEE4271D-9535-4907-B2D0-C9C19E933E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>button1</t>
   </si>
@@ -51,6 +51,42 @@
   </si>
   <si>
     <t>// 0 == not pressed    // 1 == short press    // 2 == long press    // 3 == double short press</t>
+  </si>
+  <si>
+    <t>modulo</t>
+  </si>
+  <si>
+    <t>pageID</t>
+  </si>
+  <si>
+    <t>Nom Page</t>
+  </si>
+  <si>
+    <t>0 : Home Page</t>
+  </si>
+  <si>
+    <t>1 : Ride Page</t>
+  </si>
+  <si>
+    <t>2 : Ride Statistics Page</t>
+  </si>
+  <si>
+    <t>3 : Compass Page</t>
+  </si>
+  <si>
+    <t>4 : Ride Direction Page</t>
+  </si>
+  <si>
+    <t>5 : Global Statistics Page</t>
+  </si>
+  <si>
+    <t>6 : Go Home Page</t>
+  </si>
+  <si>
+    <t>-1 : Init TS Page</t>
+  </si>
+  <si>
+    <t>-2 : No Page (error)</t>
   </si>
 </sst>
 </file>
@@ -132,11 +168,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -148,6 +181,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,34 +510,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C28F889-EB9D-470C-A8BB-EAC71480EC36}">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -508,18 +546,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
@@ -531,20 +569,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D27" si="0">B9*$B$6+C9*$C$6</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+        <f t="shared" ref="D9:D23" si="0">B9*$B$6+C9*$C$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
         <v>2</v>
       </c>
       <c r="C10">
@@ -555,8 +593,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
         <v>3</v>
       </c>
       <c r="C11">
@@ -567,11 +605,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12">
@@ -579,11 +617,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
         <v>1</v>
       </c>
       <c r="D13">
@@ -591,124 +629,234 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
-        <v>3</v>
-      </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="8">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>2</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5">
-        <v>2</v>
-      </c>
-      <c r="D17" s="8">
+      <c r="K16" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
-        <v>2</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4">
         <v>2</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
-        <v>3</v>
-      </c>
-      <c r="C19" s="5">
-        <v>2</v>
-      </c>
-      <c r="D19" s="8">
+      <c r="J18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>MOD(K19,$K$17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>3</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6">
-        <v>3</v>
-      </c>
-      <c r="D21" s="8">
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f>MOD(K20,$K$17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
-        <v>2</v>
-      </c>
-      <c r="C22" s="6">
-        <v>3</v>
-      </c>
-      <c r="D22" s="8">
+      <c r="J21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <f>MOD(K21,$K$17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3</v>
+      </c>
+      <c r="D22" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
-        <v>3</v>
-      </c>
-      <c r="C23" s="6">
-        <v>3</v>
-      </c>
-      <c r="D23" s="8">
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <f>MOD(K22,$K$17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3</v>
+      </c>
+      <c r="D23" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <f>MOD(K23,$K$17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="L24">
+        <f>MOD(K24,$K$17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25">
+        <v>6</v>
+      </c>
+      <c r="L25">
+        <f>MOD(K25,$K$17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26">
+        <v>-1</v>
+      </c>
+      <c r="L26">
+        <f>MOD(K26,$K$17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27">
+        <v>-2</v>
+      </c>
+      <c r="L27">
+        <f>MOD(K27,$K$17)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>